<commit_message>
crear usuarios y personas con excel
</commit_message>
<xml_diff>
--- a/ApiGateway/ApiGatewayExpedientes/public/formato_personas.xlsx.xlsx
+++ b/ApiGateway/ApiGatewayExpedientes/public/formato_personas.xlsx.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EF3201-1C59-4681-9919-7AA27AEAA57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="20000" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Estudiantes" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Docentes-Conciliadores" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Administrativos" state="visible" r:id="rId6"/>
+    <sheet name="Administrativos" sheetId="1" r:id="rId1"/>
+    <sheet name="Docentes-Conciliadores" sheetId="2" r:id="rId2"/>
+    <sheet name="Estudiantes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Nombres</t>
   </si>
@@ -34,37 +35,78 @@
   </si>
   <si>
     <t>Tarjeta_Profesinal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jairo </t>
+  </si>
+  <si>
+    <t>Urrego</t>
+  </si>
+  <si>
+    <t>jairo.ug@ugc.edu.co</t>
+  </si>
+  <si>
+    <t>Goku</t>
+  </si>
+  <si>
+    <t>Saiyajin</t>
+  </si>
+  <si>
+    <t>goku@ugc.edu.co</t>
+  </si>
+  <si>
+    <t>Vegeta</t>
+  </si>
+  <si>
+    <t>vegeta.ug@ugc.edu.co</t>
+  </si>
+  <si>
+    <t>Bulma</t>
+  </si>
+  <si>
+    <t>Capsula</t>
+  </si>
+  <si>
+    <t>bulma@ugc.edu.co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <color rgb="00913D"/>
+      <sz val="14"/>
+      <color rgb="FF00913D"/>
+      <name val="FrankRuehl"/>
       <family val="4"/>
-      <sz val="14"/>
-      <name val="FrankRuehl"/>
     </font>
     <font>
-      <color rgb="000000"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="FrankRuehl"/>
       <family val="4"/>
-      <sz val="14"/>
-      <name val="FrankRuehl"/>
     </font>
     <font>
-      <color rgb="00460F"/>
+      <sz val="14"/>
+      <color rgb="FF00460F"/>
+      <name val="FrankRuehl"/>
       <family val="4"/>
-      <sz val="14"/>
-      <name val="FrankRuehl"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,17 +126,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -115,8 +166,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,25 +506,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <tabColor rgb="00913D"/>
+    <tabColor rgb="FF00913D"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="20.64" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.64" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.64" style="1" customWidth="1"/>
+    <col min="1" max="2" width="20.6328125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -488,33 +541,53 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1">
+        <v>52650</v>
+      </c>
+      <c r="D2" s="1">
+        <v>321321654</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{1B72BB5E-9EED-4294-996E-D09F58024E2D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
-    <tabColor rgb="000000"/>
+    <tabColor rgb="FF000000"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="20.64" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.64" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.64" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.64" style="1" customWidth="1"/>
+    <col min="1" max="2" width="20.6328125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -534,32 +607,55 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3546231</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3142169745</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1">
+        <v>423423</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{E327F357-CC0B-4B41-8382-A8A62B53CC9A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
-    <tabColor rgb="00460F"/>
+    <tabColor rgb="FF00460F"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="20.64" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.64" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.64" style="1" customWidth="1"/>
+    <col min="1" max="2" width="20.6328125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -574,10 +670,44 @@
       </c>
       <c r="E1" s="7" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>52650</v>
+      </c>
+      <c r="D2" s="1">
+        <v>31421697</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>20252285</v>
+      </c>
+      <c r="D3" s="1">
+        <v>789524324</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Crear Usuario Lista y codificacion con manejo de errores del archivo excel
</commit_message>
<xml_diff>
--- a/ApiGateway/ApiGatewayExpedientes/public/formato_personas.xlsx.xlsx
+++ b/ApiGateway/ApiGatewayExpedientes/public/formato_personas.xlsx.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EF3201-1C59-4681-9919-7AA27AEAA57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1633A2C-42FE-462D-86A5-CF36673705F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Administrativos" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>Nombres</t>
   </si>
@@ -37,44 +37,38 @@
     <t>Tarjeta_Profesinal</t>
   </si>
   <si>
-    <t xml:space="preserve">Jairo </t>
-  </si>
-  <si>
-    <t>Urrego</t>
-  </si>
-  <si>
-    <t>jairo.ug@ugc.edu.co</t>
+    <t>Sayajin</t>
+  </si>
+  <si>
+    <t>goten@ugc.edu.co</t>
+  </si>
+  <si>
+    <t>Roshi</t>
+  </si>
+  <si>
+    <t>Krilin</t>
+  </si>
+  <si>
+    <t>Aprendiz</t>
+  </si>
+  <si>
+    <t>krilin@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son </t>
   </si>
   <si>
     <t>Goku</t>
   </si>
   <si>
-    <t>Saiyajin</t>
-  </si>
-  <si>
-    <t>goku@ugc.edu.co</t>
-  </si>
-  <si>
-    <t>Vegeta</t>
-  </si>
-  <si>
-    <t>vegeta.ug@ugc.edu.co</t>
-  </si>
-  <si>
-    <t>Bulma</t>
-  </si>
-  <si>
-    <t>Capsula</t>
-  </si>
-  <si>
-    <t>bulma@ugc.edu.co</t>
+    <t>son.goku@ugc.edu.co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,19 +78,7 @@
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FF00913D"/>
-      <name val="FrankRuehl"/>
-      <family val="4"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="FrankRuehl"/>
-      <family val="4"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF00460F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="FrankRuehl"/>
       <family val="4"/>
     </font>
@@ -109,12 +91,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00913D"/>
+        <bgColor rgb="FF00913D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00460F"/>
+        <bgColor rgb="FF00460F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5C9E31"/>
+        <bgColor rgb="FF5C9E31"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -143,36 +143,52 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB7DEE8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB7DEE8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB7DEE8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -514,7 +530,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,24 +559,29 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1249239</v>
+      </c>
+      <c r="D2" s="1">
+        <v>314439376</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1">
-        <v>52650</v>
-      </c>
-      <c r="D2" s="1">
-        <v>321321654</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:E41">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
+      <formula>LEN(TRIM(A2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{1B72BB5E-9EED-4294-996E-D09F58024E2D}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{A6BC1DFA-9EF3-4450-AE7D-C138B327AF5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
@@ -570,13 +591,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
-    <tabColor rgb="FF000000"/>
+    <tabColor rgb="FF00460F"/>
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -587,49 +608,51 @@
     <col min="6" max="6" width="20.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1">
-        <v>3546231</v>
+        <v>123456789</v>
       </c>
       <c r="D2" s="1">
-        <v>3142169745</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1">
-        <v>423423</v>
+        <v>12345675</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:E41">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(A2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{E327F357-CC0B-4B41-8382-A8A62B53CC9A}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{F7483544-50A3-41BE-8F95-42506256C80B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
@@ -639,13 +662,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
-    <tabColor rgb="FF00460F"/>
+    <tabColor rgb="FF5C9E31"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O27" sqref="O27"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -655,58 +678,49 @@
     <col min="5" max="5" width="25.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
-        <v>52650</v>
+        <v>1298323</v>
       </c>
       <c r="D2" s="1">
-        <v>31421697</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1">
-        <v>20252285</v>
-      </c>
-      <c r="D3" s="1">
-        <v>789524324</v>
-      </c>
-      <c r="E3" s="1" t="s">
+        <v>8329842</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:E41">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(A2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{B19FAFB2-7310-414D-8DE3-C174FAD3C3F3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>

</xml_diff>

<commit_message>
ajustes personas excel y modificar persona
</commit_message>
<xml_diff>
--- a/ApiGateway/ApiGatewayExpedientes/public/formato_personas.xlsx.xlsx
+++ b/ApiGateway/ApiGatewayExpedientes/public/formato_personas.xlsx.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EF3201-1C59-4681-9919-7AA27AEAA57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1633A2C-42FE-462D-86A5-CF36673705F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Administrativos" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>Nombres</t>
   </si>
@@ -37,44 +37,38 @@
     <t>Tarjeta_Profesinal</t>
   </si>
   <si>
-    <t xml:space="preserve">Jairo </t>
-  </si>
-  <si>
-    <t>Urrego</t>
-  </si>
-  <si>
-    <t>jairo.ug@ugc.edu.co</t>
+    <t>Sayajin</t>
+  </si>
+  <si>
+    <t>goten@ugc.edu.co</t>
+  </si>
+  <si>
+    <t>Roshi</t>
+  </si>
+  <si>
+    <t>Krilin</t>
+  </si>
+  <si>
+    <t>Aprendiz</t>
+  </si>
+  <si>
+    <t>krilin@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Son </t>
   </si>
   <si>
     <t>Goku</t>
   </si>
   <si>
-    <t>Saiyajin</t>
-  </si>
-  <si>
-    <t>goku@ugc.edu.co</t>
-  </si>
-  <si>
-    <t>Vegeta</t>
-  </si>
-  <si>
-    <t>vegeta.ug@ugc.edu.co</t>
-  </si>
-  <si>
-    <t>Bulma</t>
-  </si>
-  <si>
-    <t>Capsula</t>
-  </si>
-  <si>
-    <t>bulma@ugc.edu.co</t>
+    <t>son.goku@ugc.edu.co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,19 +78,7 @@
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FF00913D"/>
-      <name val="FrankRuehl"/>
-      <family val="4"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="FrankRuehl"/>
-      <family val="4"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF00460F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="FrankRuehl"/>
       <family val="4"/>
     </font>
@@ -109,12 +91,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00913D"/>
+        <bgColor rgb="FF00913D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00460F"/>
+        <bgColor rgb="FF00460F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5C9E31"/>
+        <bgColor rgb="FF5C9E31"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -143,36 +143,52 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB7DEE8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB7DEE8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFB7DEE8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -514,7 +530,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,24 +559,29 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1249239</v>
+      </c>
+      <c r="D2" s="1">
+        <v>314439376</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1">
-        <v>52650</v>
-      </c>
-      <c r="D2" s="1">
-        <v>321321654</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:E41">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
+      <formula>LEN(TRIM(A2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{1B72BB5E-9EED-4294-996E-D09F58024E2D}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{A6BC1DFA-9EF3-4450-AE7D-C138B327AF5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
@@ -570,13 +591,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
-    <tabColor rgb="FF000000"/>
+    <tabColor rgb="FF00460F"/>
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -587,49 +608,51 @@
     <col min="6" max="6" width="20.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1">
-        <v>3546231</v>
+        <v>123456789</v>
       </c>
       <c r="D2" s="1">
-        <v>3142169745</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1">
-        <v>423423</v>
+        <v>12345675</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:E41">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(A2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{E327F357-CC0B-4B41-8382-A8A62B53CC9A}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{F7483544-50A3-41BE-8F95-42506256C80B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
@@ -639,13 +662,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
-    <tabColor rgb="FF00460F"/>
+    <tabColor rgb="FF5C9E31"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O27" sqref="O27"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -655,58 +678,49 @@
     <col min="5" max="5" width="25.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
-        <v>52650</v>
+        <v>1298323</v>
       </c>
       <c r="D2" s="1">
-        <v>31421697</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1">
-        <v>20252285</v>
-      </c>
-      <c r="D3" s="1">
-        <v>789524324</v>
-      </c>
-      <c r="E3" s="1" t="s">
+        <v>8329842</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:E41">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(A2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{B19FAFB2-7310-414D-8DE3-C174FAD3C3F3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>

</xml_diff>